<commit_message>
agora ta mais especifico
</commit_message>
<xml_diff>
--- a/Cronograma de Tarefas.xlsx
+++ b/Cronograma de Tarefas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
   <si>
     <t xml:space="preserve">Segunda </t>
   </si>
@@ -121,6 +121,9 @@
   </si>
   <si>
     <t>recepcao@novahparticipacoes.com.br</t>
+  </si>
+  <si>
+    <t>seu maluco</t>
   </si>
 </sst>
 </file>
@@ -976,8 +979,8 @@
       <c r="D3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="6">
-        <v>587</v>
+      <c r="E3" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>

</xml_diff>